<commit_message>
Copy client + work list + telegram bot zayavki
</commit_message>
<xml_diff>
--- a/media/akm_download_fiz.xlsx
+++ b/media/akm_download_fiz.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vladislavkateryushin/Documents/crm-ktsNew-test/media/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{407389C3-0B3C-034B-97EB-25C7FD66427C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2841BFA0-94B9-5E48-B90B-EB176BFFD2FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="29040" windowHeight="15720" xr2:uid="{DF9E47F1-4587-4E98-94C9-887045700904}"/>
   </bookViews>
@@ -1110,13 +1110,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B7BF2C4-235C-4177-AAA8-14AEAF9D0787}">
   <dimension ref="A1:Q529"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" topLeftCell="A312" workbookViewId="0">
+      <selection activeCell="A312" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="0" hidden="1" customWidth="1"/>
+    <col min="1" max="2" width="8.83203125" style="111"/>
+    <col min="3" max="3" width="0" style="111" hidden="1" customWidth="1"/>
+    <col min="4" max="16384" width="8.83203125" style="111"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.2">
@@ -6166,7 +6168,7 @@
       <c r="P263" s="34"/>
       <c r="Q263" s="49"/>
     </row>
-    <row r="264" spans="1:17" s="111" customFormat="1" ht="14" x14ac:dyDescent="0.2">
+    <row r="264" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A264" s="17"/>
       <c r="B264" s="58"/>
       <c r="C264" s="6"/>

</xml_diff>